<commit_message>
Added 4 new plants
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9107B5A-2DD3-4DCE-96AE-CAEB1C43C3EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C29D25-BD40-4F67-BA68-00FAB12EB7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Plant</t>
   </si>
@@ -87,16 +87,96 @@
   </si>
   <si>
     <t>Level</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Level 5</t>
+  </si>
+  <si>
+    <t>Level 6</t>
+  </si>
+  <si>
+    <t>Level 0</t>
+  </si>
+  <si>
+    <t>roseberry</t>
+  </si>
+  <si>
+    <t>giraffe</t>
+  </si>
+  <si>
+    <t>bamboo</t>
+  </si>
+  <si>
+    <t>berry_bush</t>
+  </si>
+  <si>
+    <t>kitty</t>
+  </si>
+  <si>
+    <t>marijuana</t>
+  </si>
+  <si>
+    <t>pink_daisy</t>
+  </si>
+  <si>
+    <t>blue_daisy</t>
+  </si>
+  <si>
+    <t>cactus</t>
+  </si>
+  <si>
+    <t>eggplant</t>
+  </si>
+  <si>
+    <t>rose</t>
+  </si>
+  <si>
+    <t>pumpkin</t>
+  </si>
+  <si>
+    <t>bonsai</t>
+  </si>
+  <si>
+    <t>mushroom</t>
+  </si>
+  <si>
+    <t>sunflower</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,9 +202,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B506C8A2-CFE7-48E4-9F0A-C9D1E39EA76C}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,44 +535,66 @@
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="18" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -526,8 +629,29 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -564,9 +688,26 @@
         <f t="shared" ref="J3:J8" si="5">C3/F3</f>
         <v>9.0909090909090917</v>
       </c>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -603,9 +744,15 @@
         <f t="shared" si="5"/>
         <v>20.220588235294116</v>
       </c>
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
       <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -644,7 +791,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -683,7 +830,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -722,7 +869,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -761,33 +908,35 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="P16" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{24FA66D5-1237-46EC-8394-D06F3693FC78}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update balancing Excel file
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65819BE3-A2E8-4D88-B5ED-94B78CEEF29F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4C8648-5040-4FC3-83F4-0668F145E166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="1" r:id="rId1"/>
@@ -613,15 +613,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B506C8A2-CFE7-48E4-9F0A-C9D1E39EA76C}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.5703125" customWidth="1"/>
@@ -1133,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064E1270-E89F-4488-AF87-FAB220BD6EFC}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -1253,19 +1253,19 @@
         <v>3</v>
       </c>
       <c r="F2" s="1">
-        <f>AVERAGE(D2:E2)</f>
+        <f t="shared" ref="F2:F8" si="0">AVERAGE(D2:E2)</f>
         <v>4</v>
       </c>
       <c r="G2">
-        <f>D2-E2</f>
+        <f t="shared" ref="G2:G8" si="1">D2-E2</f>
         <v>2</v>
       </c>
       <c r="H2" s="1">
-        <f>F2*5</f>
+        <f t="shared" ref="H2:H8" si="2">F2*5</f>
         <v>20</v>
       </c>
       <c r="I2" s="1">
-        <f>5*H2</f>
+        <f t="shared" ref="I2:I8" si="3">5*H2</f>
         <v>100</v>
       </c>
       <c r="J2">
@@ -1280,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <f>(I2/4)*G2</f>
+        <f t="shared" ref="C3:C8" si="4">(I2/4)*G2</f>
         <v>50</v>
       </c>
       <c r="D3">
@@ -1290,23 +1290,23 @@
         <v>3</v>
       </c>
       <c r="F3" s="1">
-        <f>AVERAGE(D3:E3)</f>
+        <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
       <c r="G3">
-        <f>D3-E3</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H3" s="1">
-        <f>F3*5</f>
+        <f t="shared" si="2"/>
         <v>27.5</v>
       </c>
       <c r="I3" s="1">
-        <f>5*H3</f>
+        <f t="shared" si="3"/>
         <v>137.5</v>
       </c>
       <c r="J3" s="1">
-        <f>C3/F3</f>
+        <f t="shared" ref="J3:J8" si="5">C3/F3</f>
         <v>9.0909090909090917</v>
       </c>
     </row>
@@ -1318,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <f>(I3/4)*G3</f>
+        <f t="shared" si="4"/>
         <v>171.875</v>
       </c>
       <c r="D4">
@@ -1328,23 +1328,23 @@
         <v>5</v>
       </c>
       <c r="F4" s="1">
-        <f>AVERAGE(D4:E4)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="G4">
-        <f>D4-E4</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H4" s="1">
-        <f>F4*5</f>
+        <f t="shared" si="2"/>
         <v>42.5</v>
       </c>
       <c r="I4" s="1">
-        <f>5*H4</f>
+        <f t="shared" si="3"/>
         <v>212.5</v>
       </c>
       <c r="J4" s="1">
-        <f>C4/F4</f>
+        <f t="shared" si="5"/>
         <v>20.220588235294116</v>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <f>(I4/4)*G4</f>
+        <f t="shared" si="4"/>
         <v>371.875</v>
       </c>
       <c r="D5">
@@ -1366,23 +1366,23 @@
         <v>8</v>
       </c>
       <c r="F5" s="1">
-        <f>AVERAGE(D5:E5)</f>
+        <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
       <c r="G5">
-        <f>D5-E5</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H5" s="1">
-        <f>F5*5</f>
+        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="I5" s="1">
-        <f>5*H5</f>
+        <f t="shared" si="3"/>
         <v>287.5</v>
       </c>
       <c r="J5" s="1">
-        <f>C5/F5</f>
+        <f t="shared" si="5"/>
         <v>32.336956521739133</v>
       </c>
     </row>
@@ -1394,7 +1394,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1">
-        <f>(I5/4)*G5</f>
+        <f t="shared" si="4"/>
         <v>503.125</v>
       </c>
       <c r="D6">
@@ -1404,23 +1404,23 @@
         <v>15</v>
       </c>
       <c r="F6" s="1">
-        <f>AVERAGE(D6:E6)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="G6">
-        <f>D6-E6</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="H6" s="1">
-        <f>F6*5</f>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="I6" s="1">
-        <f>5*H6</f>
+        <f t="shared" si="3"/>
         <v>475</v>
       </c>
       <c r="J6" s="1">
-        <f>C6/F6</f>
+        <f t="shared" si="5"/>
         <v>26.480263157894736</v>
       </c>
     </row>
@@ -1432,7 +1432,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <f>(I6/4)*G6</f>
+        <f t="shared" si="4"/>
         <v>950</v>
       </c>
       <c r="D7">
@@ -1442,23 +1442,23 @@
         <v>15</v>
       </c>
       <c r="F7" s="1">
-        <f>AVERAGE(D7:E7)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G7">
-        <f>D7-E7</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="H7" s="1">
-        <f>F7*5</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="I7" s="1">
-        <f>5*H7</f>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
       <c r="J7" s="1">
-        <f>C7/F7</f>
+        <f t="shared" si="5"/>
         <v>47.5</v>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <f>(I7/4)*G7</f>
+        <f t="shared" si="4"/>
         <v>1250</v>
       </c>
       <c r="D8">
@@ -1480,23 +1480,23 @@
         <v>16</v>
       </c>
       <c r="F8" s="1">
-        <f>AVERAGE(D8:E8)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="G8">
-        <f>D8-E8</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="H8" s="1">
-        <f>F8*5</f>
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
       <c r="I8" s="1">
-        <f>5*H8</f>
+        <f t="shared" si="3"/>
         <v>575</v>
       </c>
       <c r="J8" s="1">
-        <f>C8/F8</f>
+        <f t="shared" si="5"/>
         <v>54.347826086956523</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add support for plants that overlay the pot
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF442D0-D164-41C4-9352-745DF74C0096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B69CDC-9CC1-4BB5-B985-BA4B698CB19C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
+    <workbookView xWindow="33975" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Working" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracking!$A$1:$F$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracking!$A$1:$F$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>Plant</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>Luisdenpixel</t>
+  </si>
+  <si>
+    <t>sunplant</t>
   </si>
 </sst>
 </file>
@@ -617,7 +620,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23:I23"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +747,7 @@
         <v>28</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="M3" t="s">
         <v>35</v>
@@ -782,6 +785,9 @@
       <c r="L4" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="M4" t="s">
+        <v>38</v>
+      </c>
       <c r="N4" t="s">
         <v>36</v>
       </c>
@@ -960,7 +966,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
@@ -1106,6 +1112,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
       <c r="B20" t="s">
         <v>56</v>
       </c>
@@ -1116,6 +1125,12 @@
       <c r="D20" s="6">
         <v>16</v>
       </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -1130,7 +1145,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F18" xr:uid="{DE796829-81F8-4DDB-A026-28A5EA19C969}">
+  <autoFilter ref="A1:F21" xr:uid="{DE796829-81F8-4DDB-A026-28A5EA19C969}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
       <sortCondition ref="E1:E18"/>
     </sortState>
@@ -1139,7 +1154,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E19">
+  <conditionalFormatting sqref="E2:E20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Oh shit I need to make the available plants in the shop have a longer character limit
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B69CDC-9CC1-4BB5-B985-BA4B698CB19C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DB65E9-BD40-4340-A8F2-E3CE49FA5B6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33975" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Have level 0 flowers also appear in the store as a choice from the database
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DB65E9-BD40-4340-A8F2-E3CE49FA5B6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1C1B6E-10DE-457A-AAD4-BA364737A197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33975" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
   <si>
     <t>Plant</t>
   </si>
@@ -233,6 +233,27 @@
   </si>
   <si>
     <t>sunplant</t>
+  </si>
+  <si>
+    <t>hibiscus</t>
+  </si>
+  <si>
+    <t>iris</t>
+  </si>
+  <si>
+    <t>peony</t>
+  </si>
+  <si>
+    <t>calla_lily</t>
+  </si>
+  <si>
+    <t>peace_lily</t>
+  </si>
+  <si>
+    <t>venus_flytrap</t>
+  </si>
+  <si>
+    <t>daisy_patch</t>
   </si>
 </sst>
 </file>
@@ -617,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B506C8A2-CFE7-48E4-9F0A-C9D1E39EA76C}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,6 +758,9 @@
       <c r="F3" s="1">
         <v>6</v>
       </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
       <c r="I3" t="s">
         <v>37</v>
       </c>
@@ -776,8 +800,14 @@
       <c r="F4" s="1">
         <v>6</v>
       </c>
+      <c r="H4" t="s">
+        <v>71</v>
+      </c>
       <c r="I4" t="s">
         <v>51</v>
+      </c>
+      <c r="J4" t="s">
+        <v>68</v>
       </c>
       <c r="K4" t="s">
         <v>33</v>
@@ -812,7 +842,18 @@
       <c r="F5" s="1">
         <v>7</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="I5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" t="s">
+        <v>70</v>
+      </c>
       <c r="N5" t="s">
         <v>39</v>
       </c>
@@ -1048,7 +1089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1069,7 +1110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1090,7 +1131,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1111,7 +1152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1132,7 +1173,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
       <c r="B21" t="s">
         <v>63</v>
       </c>
@@ -1142,6 +1186,159 @@
       </c>
       <c r="D21" s="6">
         <v>12</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>7</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D22" s="6">
+        <v>16</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D23" s="6">
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D24" s="6">
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D25" s="6">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>7</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D26" s="6">
+        <v>16</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1">
+        <v>7</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D27" s="6">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27" s="1">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1154,7 +1351,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E20">
+  <conditionalFormatting sqref="E2:E23">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Update the balancing Excel file
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1C1B6E-10DE-457A-AAD4-BA364737A197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B596C74D-6E32-4C0A-946F-9362D6605037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
@@ -740,23 +740,23 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B3,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B3,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D3" s="6">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H3" t="s">
         <v>66</v>
@@ -782,23 +782,23 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C4" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D4" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
         <v>71</v>
@@ -824,23 +824,23 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D5" s="6">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" t="s">
         <v>65</v>
@@ -860,62 +860,62 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
       </c>
       <c r="C6" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D6" s="6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C7" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B7,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B7,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D7" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C8" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D8" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1">
         <v>7</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
+        <v>26</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C9" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
@@ -936,15 +936,15 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9" s="1">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
@@ -957,39 +957,39 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C11" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D11" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
@@ -999,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1">
         <v>7</v>
@@ -1007,41 +1007,41 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C13" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D13" s="6">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C14" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D14" s="6">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1">
         <v>7</v>
@@ -1049,49 +1049,49 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C15" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B15,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B15,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D15" s="6">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F15" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B16,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B16,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D16" s="6">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
@@ -1104,67 +1104,67 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F17" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C18" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D18" s="6">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1">
         <v>6</v>
       </c>
-      <c r="F18" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C19" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D19" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F19" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C20" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D20" s="6">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E20">
         <v>5</v>
@@ -1173,33 +1173,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C21" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B21,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B21,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D21" s="6">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F21" s="1">
-        <v>7</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
         <v>56</v>
@@ -1212,18 +1209,15 @@
         <v>16</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F22" s="1">
         <v>7</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
         <v>56</v>
@@ -1236,122 +1230,107 @@
         <v>16</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F23" s="1">
         <v>7</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C24" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D24" s="6">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" s="1">
-        <v>7</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C25" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D25" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F25" s="1">
-        <v>7</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C26" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D26" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F26" s="1">
         <v>7</v>
       </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C27" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D27" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F27" s="1">
-        <v>7</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F21" xr:uid="{DE796829-81F8-4DDB-A026-28A5EA19C969}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
-      <sortCondition ref="E1:E18"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F27">
+      <sortCondition ref="E1:E21"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F18">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E23">
+  <conditionalFormatting sqref="E2:E230">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Add a cool new plant from Parker
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B596C74D-6E32-4C0A-946F-9362D6605037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BA9C3D-E4B3-4089-AA07-971CE4095FBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
   <si>
     <t>Plant</t>
   </si>
@@ -254,6 +254,15 @@
   </si>
   <si>
     <t>daisy_patch</t>
+  </si>
+  <si>
+    <t>dandelion</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>Discord</t>
   </si>
 </sst>
 </file>
@@ -638,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B506C8A2-CFE7-48E4-9F0A-C9D1E39EA76C}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,23 +707,23 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
+        <v>26</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B2,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B2,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <f>IF(_xlfn.XLOOKUP(B2,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B2,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
       </c>
       <c r="D2" s="6">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -740,23 +749,23 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B3,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B3,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <f>IF(_xlfn.XLOOKUP(B3,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B3,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
       </c>
       <c r="D3" s="6">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
         <v>66</v>
@@ -782,23 +791,23 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C4" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <f>IF(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
       </c>
       <c r="D4" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
       </c>
       <c r="H4" t="s">
         <v>71</v>
@@ -824,27 +833,30 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C5" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <f>IF(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
       </c>
       <c r="D5" s="6">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I5" t="s">
         <v>65</v>
       </c>
+      <c r="J5" t="s">
+        <v>72</v>
+      </c>
       <c r="K5" t="s">
         <v>69</v>
       </c>
@@ -860,41 +872,41 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C6" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D6" s="6">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C7" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B7,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B7,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B7,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B7,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D7" s="6">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1">
         <v>7</v>
@@ -902,17 +914,17 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C8" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D8" s="6">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -923,62 +935,62 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
       </c>
       <c r="C9" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <f>IF(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
       </c>
       <c r="D9" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C10" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B10,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B10,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <f>IF(_xlfn.XLOOKUP(B10,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B10,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
       </c>
       <c r="D10" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" s="1">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C11" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <f>IF(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
       </c>
       <c r="D11" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1">
         <v>7</v>
@@ -986,13 +998,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v/>
       </c>
       <c r="D12" s="6">
@@ -1007,13 +1019,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C13" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v/>
       </c>
       <c r="D13" s="6">
@@ -1028,17 +1040,17 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C14" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <f>IF(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
       </c>
       <c r="D14" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -1049,20 +1061,20 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B15,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B15,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <f>IF(_xlfn.XLOOKUP(B15,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B15,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
       </c>
       <c r="D15" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F15" s="1">
         <v>7</v>
@@ -1070,41 +1082,41 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C16" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B16,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B16,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <f>IF(_xlfn.XLOOKUP(B16,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B16,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
       </c>
       <c r="D16" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E16">
         <v>4</v>
       </c>
-      <c r="F16">
-        <v>8</v>
+      <c r="F16" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C17" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B17,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B17,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <f>IF(_xlfn.XLOOKUP(B17,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B17,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
       </c>
       <c r="D17" s="6">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F17" s="1">
         <v>7</v>
@@ -1112,41 +1124,41 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C18" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D18" s="6">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D19" s="6">
         <v>16</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" s="1">
         <v>7</v>
@@ -1154,20 +1166,20 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C20" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <f>IF(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
       </c>
       <c r="D20" s="6">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F20" s="1">
         <v>7</v>
@@ -1175,128 +1187,128 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B21,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B21,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B21,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B21,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D21" s="6">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E21">
-        <v>5</v>
-      </c>
-      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C22" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D22" s="6">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F22" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C23" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D23" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F23" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D24" s="6">
         <v>24</v>
       </c>
       <c r="E24">
-        <v>6</v>
-      </c>
-      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="F24" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C25" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <f>IF(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
       </c>
       <c r="D25" s="6">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25" s="1">
         <v>6</v>
-      </c>
-      <c r="F25" s="1">
-        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C26" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
-        <v/>
+        <f>IF(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
       </c>
       <c r="D26" s="6">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E26">
         <v>6</v>
       </c>
-      <c r="F26" s="1">
-        <v>7</v>
+      <c r="F26">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1307,7 +1319,7 @@
         <v>50</v>
       </c>
       <c r="C27" s="4" t="str">
-        <f>IF(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$B$1:$B$5, ""), "Link"), "")</f>
+        <f>IF(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v/>
       </c>
       <c r="D27" s="6">
@@ -1320,10 +1332,27 @@
         <v>6</v>
       </c>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F21" xr:uid="{DE796829-81F8-4DDB-A026-28A5EA19C969}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F27">
-      <sortCondition ref="E1:E21"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
+      <sortCondition descending="1" ref="F1:F21"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F18">
@@ -1349,64 +1378,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064E1270-E89F-4488-AF87-FAB220BD6EFC}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="str">
+        <f>"375320699201650688"</f>
+        <v>375320699201650688</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{D347887C-626B-46E2-9ACA-8CFFEBA86AB8}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{1852A152-A139-404A-A721-487528C06157}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{8D140910-929B-4CCC-9E43-DEDC8A2557CE}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{C0317918-4A3D-48DA-B5F9-616B96661333}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{D347887C-626B-46E2-9ACA-8CFFEBA86AB8}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{1852A152-A139-404A-A721-487528C06157}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{8D140910-929B-4CCC-9E43-DEDC8A2557CE}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{C0317918-4A3D-48DA-B5F9-616B96661333}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new artist to the config file
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BA9C3D-E4B3-4089-AA07-971CE4095FBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65B5972-A7D2-4E27-9981-A13D36F4DE7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tracking" sheetId="1" r:id="rId1"/>
-    <sheet name="Artist Links" sheetId="3" r:id="rId2"/>
-    <sheet name="Working" sheetId="2" r:id="rId3"/>
+    <sheet name="Plant Level Tracking" sheetId="1" r:id="rId1"/>
+    <sheet name="Plant Level Tracking Overhaul" sheetId="6" r:id="rId2"/>
+    <sheet name="Artist Links" sheetId="3" r:id="rId3"/>
+    <sheet name="Exp Gain Per Water (Baseline)" sheetId="4" r:id="rId4"/>
+    <sheet name="Exp Gain Per Water (Multiple)" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracking!$A$1:$F$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plant Level Tracking'!$A$1:$F$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Plant Level Tracking Overhaul'!$A$1:$F$21</definedName>
+    <definedName name="TotalMultiplier">'Exp Gain Per Water (Multiple)'!$K$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,56 +42,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="94">
   <si>
     <t>Plant</t>
   </si>
   <si>
-    <t>Max Exp</t>
-  </si>
-  <si>
-    <t>Min Exp</t>
-  </si>
-  <si>
-    <t>Average Exp</t>
-  </si>
-  <si>
-    <t>Berry Bush</t>
-  </si>
-  <si>
-    <t>Blue Daisy</t>
-  </si>
-  <si>
-    <t>Cactus</t>
-  </si>
-  <si>
-    <t>Giraffe</t>
-  </si>
-  <si>
-    <t>Pink Daisy</t>
-  </si>
-  <si>
-    <t>Roseberry</t>
-  </si>
-  <si>
-    <t>Exp Range</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
-    <t>5 Waters</t>
-  </si>
-  <si>
-    <t>5 Plants</t>
-  </si>
-  <si>
-    <t>How many waters it takes to get another one</t>
-  </si>
-  <si>
-    <t>Bamboo</t>
-  </si>
-  <si>
     <t>Level</t>
   </si>
   <si>
@@ -263,6 +225,105 @@
   </si>
   <si>
     <t>Discord</t>
+  </si>
+  <si>
+    <t>Plant Level</t>
+  </si>
+  <si>
+    <t>Minimum Water Exp</t>
+  </si>
+  <si>
+    <t>Maximum Water Exp</t>
+  </si>
+  <si>
+    <t>Average Exp Water</t>
+  </si>
+  <si>
+    <t>Plant Level vs Plant Count</t>
+  </si>
+  <si>
+    <t>Multipliers</t>
+  </si>
+  <si>
+    <t>Total Multiplier</t>
+  </si>
+  <si>
+    <t>Level of Unlock</t>
+  </si>
+  <si>
+    <t>Plants Available</t>
+  </si>
+  <si>
+    <t>New system would have each plant give you the same amount of exp (or an amount that scales based on level but that doesn't really matter)</t>
+  </si>
+  <si>
+    <t>When you water a plant it gives you EXP and it gives you GOLD</t>
+  </si>
+  <si>
+    <t>Gold can be used to purchase new pots and new items</t>
+  </si>
+  <si>
+    <t>Exp is used to personally level up</t>
+  </si>
+  <si>
+    <t>Levelling up gives you access to the new set of plants available plants</t>
+  </si>
+  <si>
+    <t>Levelling up DOESN’T take away access to the previous level of plants</t>
+  </si>
+  <si>
+    <t>So like a level 2 person's shop would contain 3 things from the level 0 segment</t>
+  </si>
+  <si>
+    <t>A level 7's shop would contain 3 things from level 0 and 3 things from level 5</t>
+  </si>
+  <si>
+    <t>Exp and Levelling</t>
+  </si>
+  <si>
+    <t>Plants</t>
+  </si>
+  <si>
+    <t>All of the plants give an amount (N) of exp</t>
+  </si>
+  <si>
+    <t>This amount of exp will SCALE with your current level</t>
+  </si>
+  <si>
+    <t>Watering</t>
+  </si>
+  <si>
+    <t>Watering a plant will giveyou both GOLD and EXP</t>
+  </si>
+  <si>
+    <t>Exp is used for levelling</t>
+  </si>
+  <si>
+    <t>Gold is used to purhcase items</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>The shop contains available plants + available items</t>
+  </si>
+  <si>
+    <t>The plants available to you depend on your current level</t>
+  </si>
+  <si>
+    <t>You will always have revival tokens + pots available to you, but their prices depend upon your level</t>
+  </si>
+  <si>
+    <t>spruce</t>
+  </si>
+  <si>
+    <t>tomato</t>
+  </si>
+  <si>
+    <t>crocus</t>
+  </si>
+  <si>
+    <t>eucalyptus</t>
   </si>
 </sst>
 </file>
@@ -324,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -332,6 +393,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -649,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B506C8A2-CFE7-48E4-9F0A-C9D1E39EA76C}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S31" activeCellId="4" sqref="H5 J6 K6 N6 S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,48 +738,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B2,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B2,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -726,33 +795,33 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B3,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B3,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -768,33 +837,33 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="M3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -810,33 +879,33 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="M4" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -851,31 +920,34 @@
       <c r="F5" s="1">
         <v>8</v>
       </c>
+      <c r="H5" t="s">
+        <v>92</v>
+      </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="K5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="M5" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="N5" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C6" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -890,13 +962,22 @@
       <c r="F6" s="1">
         <v>7</v>
       </c>
+      <c r="J6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6" t="s">
+        <v>93</v>
+      </c>
+      <c r="N6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B7,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B7,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -914,10 +995,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C8" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -935,10 +1016,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -956,10 +1037,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C10" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B10,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B10,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -977,10 +1058,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C11" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -998,10 +1079,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C12" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1019,10 +1100,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C13" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1040,10 +1121,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C14" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1061,10 +1142,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B15,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B15,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1082,10 +1163,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C16" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B16,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B16,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1103,10 +1184,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C17" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B17,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B17,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1124,10 +1205,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C18" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1145,10 +1226,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C19" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1166,10 +1247,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C20" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1187,10 +1268,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C21" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B21,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B21,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1208,10 +1289,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C22" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1229,10 +1310,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C23" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1250,10 +1331,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C24" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1271,10 +1352,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C25" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1292,10 +1373,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C26" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1313,10 +1394,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C27" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1334,10 +1415,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D28" s="6">
         <v>0</v>
@@ -1377,6 +1458,825 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1418663-B0D9-4839-A0F9-92369B0C3610}">
+  <dimension ref="A1:O30"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B2,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B2,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D2" s="6">
+        <v>12</v>
+      </c>
+      <c r="E2" s="10">
+        <f t="shared" ref="E2:E28" si="0">VALUE(_xlfn.CONCAT(_xlfn.XLOOKUP(A2,$J$2:$J$5,$H$2:$H$5, ""), _xlfn.XLOOKUP(A2,$K$2:$K$5,$H$2:$H$5, ""), _xlfn.XLOOKUP(A2,$L$2:$L$5,$H$2:$H$5, ""), _xlfn.XLOOKUP(A2,$M$2:$M$5,$H$2:$H$5, ""), _xlfn.XLOOKUP(A2,$N$2:$N$5,$H$2:$H$5, ""), _xlfn.XLOOKUP(A2,$O$2:$O$5,$H$2:$H$5, ""), _xlfn.XLOOKUP(A2,$I$2:$I$5,$H$2:$H$5, "")))</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B3,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B3,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D3" s="6">
+        <v>16</v>
+      </c>
+      <c r="E3" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D5" s="6">
+        <v>16</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>7</v>
+      </c>
+      <c r="H5" s="2">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D6" s="6">
+        <v>32</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B7,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B7,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D7" s="6">
+        <v>24</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B10,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B10,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D11" s="6">
+        <v>16</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>7</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
+      </c>
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>7</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>7</v>
+      </c>
+      <c r="H14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6</v>
+      </c>
+      <c r="H15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B16,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B16,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
+      </c>
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B17,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B17,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D17" s="6">
+        <v>16</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F17" s="1">
+        <v>7</v>
+      </c>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
+      </c>
+      <c r="D18" s="6">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F18" s="1">
+        <v>7</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D19" s="6">
+        <v>16</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F19" s="1">
+        <v>7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D20" s="6">
+        <v>32</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F20" s="1">
+        <v>7</v>
+      </c>
+      <c r="H20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B21,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B21,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D21" s="6">
+        <v>24</v>
+      </c>
+      <c r="E21" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F21" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D22" s="6">
+        <v>24</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F22" s="1">
+        <v>6</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
+      </c>
+      <c r="D23" s="6">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F23" s="1">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B24,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D24" s="6">
+        <v>16</v>
+      </c>
+      <c r="E24" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F24" s="1">
+        <v>7</v>
+      </c>
+      <c r="H24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B25,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D25" s="6">
+        <v>16</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F25" s="1">
+        <v>7</v>
+      </c>
+      <c r="H25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
+      </c>
+      <c r="D26" s="6">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F26" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v>Link</v>
+      </c>
+      <c r="D27" s="6">
+        <v>24</v>
+      </c>
+      <c r="E27" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="4" t="str">
+        <f>IF(_xlfn.XLOOKUP(B28,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B28,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
+        <v/>
+      </c>
+      <c r="D28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F28" s="1">
+        <v>6</v>
+      </c>
+      <c r="H28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F21" xr:uid="{DE796829-81F8-4DDB-A026-28A5EA19C969}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
+      <sortCondition ref="E1:E21"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="I1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064E1270-E89F-4488-AF87-FAB220BD6EFC}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1393,50 +2293,50 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B6" t="str">
         <f>"375320699201650688"</f>
@@ -1454,310 +2354,581 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370672FE-097C-4622-B4BB-552E2E08767F}">
-  <dimension ref="A1:J8"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14ABBD8F-4695-44C8-B308-5DEE8084E3A2}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <f>AVERAGE(C2:D2)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>80</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E8" si="0">AVERAGE(C3:D3)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B4">
+        <v>172</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>120</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="B5">
+        <v>372</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+      <c r="D5">
+        <v>150</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>503</v>
+      </c>
+      <c r="C6">
+        <v>150</v>
+      </c>
+      <c r="D6">
+        <v>230</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>950</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+      <c r="D7">
+        <v>250</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1250</v>
+      </c>
+      <c r="C8">
+        <v>160</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DD8FDB-DCE4-43C1-8267-23AF925CAFA9}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>_xlfn.XLOOKUP(B$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A2 * TotalMultiplier</f>
+        <v>52.800000000000004</v>
+      </c>
+      <c r="C2">
+        <f>_xlfn.XLOOKUP(C$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A2 * TotalMultiplier</f>
+        <v>72.600000000000009</v>
+      </c>
+      <c r="D2">
+        <f>_xlfn.XLOOKUP(D$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A2 * TotalMultiplier</f>
+        <v>112.2</v>
+      </c>
+      <c r="E2">
+        <f>_xlfn.XLOOKUP(E$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A2 * TotalMultiplier</f>
+        <v>151.80000000000001</v>
+      </c>
+      <c r="F2">
+        <f>_xlfn.XLOOKUP(F$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A2 * TotalMultiplier</f>
+        <v>250.8</v>
+      </c>
+      <c r="G2">
+        <f>_xlfn.XLOOKUP(G$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A2 * TotalMultiplier</f>
+        <v>264</v>
+      </c>
+      <c r="H2">
+        <f>_xlfn.XLOOKUP(H$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A2 * TotalMultiplier</f>
+        <v>303.60000000000002</v>
+      </c>
+      <c r="J2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K2">
+        <f>J2*J3*J4*J5*J6*J7*J8*J9*J10*J11</f>
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>_xlfn.XLOOKUP(B$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A3 * TotalMultiplier</f>
+        <v>105.60000000000001</v>
+      </c>
+      <c r="C3">
+        <f>_xlfn.XLOOKUP(C$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A3 * TotalMultiplier</f>
+        <v>145.20000000000002</v>
+      </c>
+      <c r="D3">
+        <f>_xlfn.XLOOKUP(D$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A3 * TotalMultiplier</f>
+        <v>224.4</v>
+      </c>
+      <c r="E3">
+        <f>_xlfn.XLOOKUP(E$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A3 * TotalMultiplier</f>
+        <v>303.60000000000002</v>
+      </c>
+      <c r="F3">
+        <f>_xlfn.XLOOKUP(F$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A3 * TotalMultiplier</f>
+        <v>501.6</v>
+      </c>
+      <c r="G3">
+        <f>_xlfn.XLOOKUP(G$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A3 * TotalMultiplier</f>
+        <v>528</v>
+      </c>
+      <c r="H3">
+        <f>_xlfn.XLOOKUP(H$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A3 * TotalMultiplier</f>
+        <v>607.20000000000005</v>
+      </c>
+      <c r="J3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>_xlfn.XLOOKUP(B$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A4 * TotalMultiplier</f>
+        <v>158.4</v>
+      </c>
+      <c r="C4">
+        <f>_xlfn.XLOOKUP(C$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A4 * TotalMultiplier</f>
+        <v>217.8</v>
+      </c>
+      <c r="D4">
+        <f>_xlfn.XLOOKUP(D$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A4 * TotalMultiplier</f>
+        <v>336.6</v>
+      </c>
+      <c r="E4">
+        <f>_xlfn.XLOOKUP(E$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A4 * TotalMultiplier</f>
+        <v>455.40000000000003</v>
+      </c>
+      <c r="F4">
+        <f>_xlfn.XLOOKUP(F$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A4 * TotalMultiplier</f>
+        <v>752.40000000000009</v>
+      </c>
+      <c r="G4">
+        <f>_xlfn.XLOOKUP(G$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A4 * TotalMultiplier</f>
+        <v>792</v>
+      </c>
+      <c r="H4">
+        <f>_xlfn.XLOOKUP(H$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A4 * TotalMultiplier</f>
+        <v>910.80000000000007</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f>_xlfn.XLOOKUP(B$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A5 * TotalMultiplier</f>
+        <v>211.20000000000002</v>
+      </c>
+      <c r="C5">
+        <f>_xlfn.XLOOKUP(C$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A5 * TotalMultiplier</f>
+        <v>290.40000000000003</v>
+      </c>
+      <c r="D5">
+        <f>_xlfn.XLOOKUP(D$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A5 * TotalMultiplier</f>
+        <v>448.8</v>
+      </c>
+      <c r="E5">
+        <f>_xlfn.XLOOKUP(E$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A5 * TotalMultiplier</f>
+        <v>607.20000000000005</v>
+      </c>
+      <c r="F5">
+        <f>_xlfn.XLOOKUP(F$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A5 * TotalMultiplier</f>
+        <v>1003.2</v>
+      </c>
+      <c r="G5">
+        <f>_xlfn.XLOOKUP(G$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A5 * TotalMultiplier</f>
+        <v>1056</v>
+      </c>
+      <c r="H5">
+        <f>_xlfn.XLOOKUP(H$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A5 * TotalMultiplier</f>
+        <v>1214.4000000000001</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f>_xlfn.XLOOKUP(B$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A6 * TotalMultiplier</f>
+        <v>264</v>
+      </c>
+      <c r="C6">
+        <f>_xlfn.XLOOKUP(C$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A6 * TotalMultiplier</f>
+        <v>363</v>
+      </c>
+      <c r="D6">
+        <f>_xlfn.XLOOKUP(D$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A6 * TotalMultiplier</f>
+        <v>561</v>
+      </c>
+      <c r="E6">
+        <f>_xlfn.XLOOKUP(E$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A6 * TotalMultiplier</f>
+        <v>759</v>
+      </c>
+      <c r="F6">
+        <f>_xlfn.XLOOKUP(F$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A6 * TotalMultiplier</f>
+        <v>1254</v>
+      </c>
+      <c r="G6">
+        <f>_xlfn.XLOOKUP(G$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A6 * TotalMultiplier</f>
+        <v>1320</v>
+      </c>
+      <c r="H6">
+        <f>_xlfn.XLOOKUP(H$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A6 * TotalMultiplier</f>
+        <v>1518</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f>_xlfn.XLOOKUP(B$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A7 * TotalMultiplier</f>
+        <v>316.8</v>
+      </c>
+      <c r="C7">
+        <f>_xlfn.XLOOKUP(C$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A7 * TotalMultiplier</f>
+        <v>435.6</v>
+      </c>
+      <c r="D7">
+        <f>_xlfn.XLOOKUP(D$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A7 * TotalMultiplier</f>
+        <v>673.2</v>
+      </c>
+      <c r="E7">
+        <f>_xlfn.XLOOKUP(E$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A7 * TotalMultiplier</f>
+        <v>910.80000000000007</v>
+      </c>
+      <c r="F7">
+        <f>_xlfn.XLOOKUP(F$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A7 * TotalMultiplier</f>
+        <v>1504.8000000000002</v>
+      </c>
+      <c r="G7">
+        <f>_xlfn.XLOOKUP(G$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A7 * TotalMultiplier</f>
+        <v>1584</v>
+      </c>
+      <c r="H7">
+        <f>_xlfn.XLOOKUP(H$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A7 * TotalMultiplier</f>
+        <v>1821.6000000000001</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f>_xlfn.XLOOKUP(B$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A8 * TotalMultiplier</f>
+        <v>369.6</v>
+      </c>
+      <c r="C8">
+        <f>_xlfn.XLOOKUP(C$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A8 * TotalMultiplier</f>
+        <v>508.20000000000005</v>
+      </c>
+      <c r="D8">
+        <f>_xlfn.XLOOKUP(D$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A8 * TotalMultiplier</f>
+        <v>785.40000000000009</v>
+      </c>
+      <c r="E8">
+        <f>_xlfn.XLOOKUP(E$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A8 * TotalMultiplier</f>
+        <v>1062.6000000000001</v>
+      </c>
+      <c r="F8">
+        <f>_xlfn.XLOOKUP(F$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A8 * TotalMultiplier</f>
+        <v>1755.6000000000001</v>
+      </c>
+      <c r="G8">
+        <f>_xlfn.XLOOKUP(G$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A8 * TotalMultiplier</f>
+        <v>1848</v>
+      </c>
+      <c r="H8">
+        <f>_xlfn.XLOOKUP(H$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A8 * TotalMultiplier</f>
+        <v>2125.2000000000003</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>_xlfn.XLOOKUP(B$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A9 * TotalMultiplier</f>
+        <v>422.40000000000003</v>
+      </c>
+      <c r="C9">
+        <f>_xlfn.XLOOKUP(C$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A9 * TotalMultiplier</f>
+        <v>580.80000000000007</v>
+      </c>
+      <c r="D9">
+        <f>_xlfn.XLOOKUP(D$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A9 * TotalMultiplier</f>
+        <v>897.6</v>
+      </c>
+      <c r="E9">
+        <f>_xlfn.XLOOKUP(E$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A9 * TotalMultiplier</f>
+        <v>1214.4000000000001</v>
+      </c>
+      <c r="F9">
+        <f>_xlfn.XLOOKUP(F$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A9 * TotalMultiplier</f>
+        <v>2006.4</v>
+      </c>
+      <c r="G9">
+        <f>_xlfn.XLOOKUP(G$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A9 * TotalMultiplier</f>
+        <v>2112</v>
+      </c>
+      <c r="H9">
+        <f>_xlfn.XLOOKUP(H$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A9 * TotalMultiplier</f>
+        <v>2428.8000000000002</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>_xlfn.XLOOKUP(B$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A10 * TotalMultiplier</f>
+        <v>475.20000000000005</v>
+      </c>
+      <c r="C10">
+        <f>_xlfn.XLOOKUP(C$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A10 * TotalMultiplier</f>
+        <v>653.4</v>
+      </c>
+      <c r="D10">
+        <f>_xlfn.XLOOKUP(D$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A10 * TotalMultiplier</f>
+        <v>1009.8000000000001</v>
+      </c>
+      <c r="E10">
+        <f>_xlfn.XLOOKUP(E$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A10 * TotalMultiplier</f>
+        <v>1366.2</v>
+      </c>
+      <c r="F10">
+        <f>_xlfn.XLOOKUP(F$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A10 * TotalMultiplier</f>
+        <v>2257.2000000000003</v>
+      </c>
+      <c r="G10">
+        <f>_xlfn.XLOOKUP(G$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A10 * TotalMultiplier</f>
+        <v>2376</v>
+      </c>
+      <c r="H10">
+        <f>_xlfn.XLOOKUP(H$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A10 * TotalMultiplier</f>
+        <v>2732.4</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1">
-        <f t="shared" ref="F2:F8" si="0">AVERAGE(D2:E2)</f>
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G8" si="1">D2-E2</f>
-        <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <f t="shared" ref="H2:H8" si="2">F2*5</f>
-        <v>20</v>
-      </c>
-      <c r="I2" s="1">
-        <f t="shared" ref="I2:I8" si="3">5*H2</f>
-        <v>100</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
+      <c r="B11">
+        <f>_xlfn.XLOOKUP(B$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A11 * TotalMultiplier</f>
+        <v>528</v>
+      </c>
+      <c r="C11">
+        <f>_xlfn.XLOOKUP(C$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A11 * TotalMultiplier</f>
+        <v>726</v>
+      </c>
+      <c r="D11">
+        <f>_xlfn.XLOOKUP(D$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A11 * TotalMultiplier</f>
+        <v>1122</v>
+      </c>
+      <c r="E11">
+        <f>_xlfn.XLOOKUP(E$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A11 * TotalMultiplier</f>
+        <v>1518</v>
+      </c>
+      <c r="F11">
+        <f>_xlfn.XLOOKUP(F$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A11 * TotalMultiplier</f>
+        <v>2508</v>
+      </c>
+      <c r="G11">
+        <f>_xlfn.XLOOKUP(G$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A11 * TotalMultiplier</f>
+        <v>2640</v>
+      </c>
+      <c r="H11">
+        <f>_xlfn.XLOOKUP(H$1, 'Exp Gain Per Water (Baseline)'!$A$2:$A$8,'Exp Gain Per Water (Baseline)'!$E$2:$E$8) * $A11 * TotalMultiplier</f>
+        <v>3036</v>
+      </c>
+      <c r="J11">
         <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <f t="shared" ref="C3:C8" si="4">(I2/4)*G2</f>
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" si="0"/>
-        <v>5.5</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="H3" s="1">
-        <f t="shared" si="2"/>
-        <v>27.5</v>
-      </c>
-      <c r="I3" s="1">
-        <f t="shared" si="3"/>
-        <v>137.5</v>
-      </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J8" si="5">C3/F3</f>
-        <v>9.0909090909090917</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" si="4"/>
-        <v>171.875</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" si="2"/>
-        <v>42.5</v>
-      </c>
-      <c r="I4" s="1">
-        <f t="shared" si="3"/>
-        <v>212.5</v>
-      </c>
-      <c r="J4" s="1">
-        <f t="shared" si="5"/>
-        <v>20.220588235294116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <f t="shared" si="4"/>
-        <v>371.875</v>
-      </c>
-      <c r="D5">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>11.5</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="H5" s="1">
-        <f t="shared" si="2"/>
-        <v>57.5</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" si="3"/>
-        <v>287.5</v>
-      </c>
-      <c r="J5" s="1">
-        <f t="shared" si="5"/>
-        <v>32.336956521739133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <f t="shared" si="4"/>
-        <v>503.125</v>
-      </c>
-      <c r="D6">
-        <v>23</v>
-      </c>
-      <c r="E6">
-        <v>15</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" si="2"/>
-        <v>95</v>
-      </c>
-      <c r="I6" s="1">
-        <f t="shared" si="3"/>
-        <v>475</v>
-      </c>
-      <c r="J6" s="1">
-        <f t="shared" si="5"/>
-        <v>26.480263157894736</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <f t="shared" si="4"/>
-        <v>950</v>
-      </c>
-      <c r="D7">
-        <v>25</v>
-      </c>
-      <c r="E7">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" si="3"/>
-        <v>500</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="5"/>
-        <v>47.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" si="4"/>
-        <v>1250</v>
-      </c>
-      <c r="D8">
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <v>16</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="2"/>
-        <v>115</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" si="3"/>
-        <v>575</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="5"/>
-        <v>54.347826086956523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make the plant pack files public
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C360F85E-2975-4C9B-A9C1-271E505DD7F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8E7F2D-454F-4E9E-B588-7920E75355A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant Level Tracking" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="121">
   <si>
     <t>Plant</t>
   </si>
@@ -348,6 +348,63 @@
   </si>
   <si>
     <t>New Exp Fraction</t>
+  </si>
+  <si>
+    <t>Nourishment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "nourishment_display_levels": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "1": 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "3": 2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "6": 3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "9": 4,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "12": 5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "15": 6,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "18": 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "2": 2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "5": 3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "15": 5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "20": 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "8": 4,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "11": 5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "13": 6,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "16": 7,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "18": 7</t>
   </si>
 </sst>
 </file>
@@ -423,10 +480,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -745,15 +802,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B506C8A2-CFE7-48E4-9F0A-C9D1E39EA76C}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.5703125" customWidth="1"/>
@@ -845,7 +902,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -858,10 +915,10 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
       </c>
       <c r="H3" t="s">
         <v>52</v>
@@ -887,23 +944,23 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B4,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D4" s="6">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
         <v>57</v>
@@ -929,23 +986,23 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C5" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B5,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D5" s="6">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>6</v>
       </c>
-      <c r="F5" s="1">
-        <v>8</v>
+      <c r="F5">
+        <v>6</v>
       </c>
       <c r="H5" t="s">
         <v>92</v>
@@ -971,20 +1028,20 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B6,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D6" s="6">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1">
         <v>7</v>
@@ -1001,7 +1058,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -1014,7 +1071,7 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1">
         <v>7</v>
@@ -1022,73 +1079,89 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B8,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D8" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="C9" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B9,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D9" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C10" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B10,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B10,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D10" s="6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <f>CEILING($K$10*I10/20, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="K10">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C11" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B11,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1098,18 +1171,25 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="1">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11:J29" si="0">CEILING($K$10*I11/20, 1)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B12,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1124,13 +1204,29 @@
       <c r="F12" s="1">
         <v>7</v>
       </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <v>7</v>
+      </c>
+      <c r="N12">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="C13" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B13,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1143,36 +1239,68 @@
         <v>3</v>
       </c>
       <c r="F13" s="1">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L13" t="s">
+        <v>103</v>
+      </c>
+      <c r="M13" t="s">
+        <v>103</v>
+      </c>
+      <c r="N13" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B14,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D14" s="6">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
         <v>7</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L14" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14" t="s">
+        <v>104</v>
+      </c>
+      <c r="N14" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B15,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B15,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1182,15 +1310,31 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F15" s="1">
         <v>7</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L15" t="s">
+        <v>105</v>
+      </c>
+      <c r="M15" t="s">
+        <v>105</v>
+      </c>
+      <c r="N15" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
@@ -1203,81 +1347,145 @@
         <v>16</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L16" t="s">
+        <v>106</v>
+      </c>
+      <c r="M16" t="s">
+        <v>106</v>
+      </c>
+      <c r="N16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C17" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B17,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B17,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D17" s="6">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L17" t="s">
+        <v>116</v>
+      </c>
+      <c r="M17" t="s">
+        <v>107</v>
+      </c>
+      <c r="N17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C18" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B18,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D18" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>9</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L18" t="s">
+        <v>117</v>
+      </c>
+      <c r="M18" t="s">
+        <v>108</v>
+      </c>
+      <c r="N18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C19" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B19,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D19" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L19" t="s">
+        <v>118</v>
+      </c>
+      <c r="M19" t="s">
+        <v>109</v>
+      </c>
+      <c r="N19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B20,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1290,12 +1498,28 @@
         <v>6</v>
       </c>
       <c r="F20" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>11</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L20" t="s">
+        <v>119</v>
+      </c>
+      <c r="M20" t="s">
+        <v>110</v>
+      </c>
+      <c r="N20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
@@ -1305,60 +1529,90 @@
         <v>Link</v>
       </c>
       <c r="D21" s="6">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>12</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L21" t="s">
+        <v>120</v>
+      </c>
+      <c r="M21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C22" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B22,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D22" s="6">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F22" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>13</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C23" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B23,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
         <v>Link</v>
       </c>
       <c r="D23" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F23" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>14</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
         <v>29</v>
@@ -1368,16 +1622,23 @@
         <v>Link</v>
       </c>
       <c r="D24" s="6">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F24" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>15</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1397,34 +1658,48 @@
       <c r="F25" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>16</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C26" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B26,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
-        <v>Link</v>
+        <v/>
       </c>
       <c r="D26" s="6">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" s="1">
+        <v>13</v>
+      </c>
+      <c r="I26">
+        <v>17</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C27" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B27,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1434,18 +1709,25 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F27" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>18</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="C28" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B28,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B28,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
@@ -1455,57 +1737,71 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>2</v>
-      </c>
-      <c r="F28" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="I28">
+        <v>19</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="C29" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B29,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B29,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D29" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F29" s="1">
+        <v>7</v>
+      </c>
+      <c r="I29">
+        <v>20</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="C30" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B30,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B30,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D30" s="6">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F30" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
         <v>94</v>
@@ -1518,37 +1814,37 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="C32" s="4" t="str">
         <f>IF(_xlfn.XLOOKUP(B32,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, "")&lt;&gt;"", HYPERLINK(_xlfn.XLOOKUP(B32,'Artist Links'!$A$1:$A$5,'Artist Links'!$C$1:$C$5, ""), "Link"), "")</f>
-        <v/>
+        <v>Link</v>
       </c>
       <c r="D32" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E32">
-        <v>6</v>
-      </c>
-      <c r="F32">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="F32" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F21" xr:uid="{DE796829-81F8-4DDB-A026-28A5EA19C969}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
-      <sortCondition descending="1" ref="F1:F21"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F32">
+      <sortCondition ref="A1:A21"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F18">
@@ -1556,6 +1852,18 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E2:E230">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:J29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1576,7 +1884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1418663-B0D9-4839-A0F9-92369B0C3610}">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K35" sqref="K35:K54"/>
     </sheetView>
   </sheetViews>
@@ -1614,15 +1922,15 @@
       <c r="H1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1645,7 +1953,7 @@
       <c r="F2" s="1">
         <v>7</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <v>0</v>
       </c>
       <c r="I2" t="s">
@@ -1691,7 +1999,7 @@
       <c r="F3" s="1">
         <v>7</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>5</v>
       </c>
       <c r="I3" t="s">
@@ -1737,7 +2045,7 @@
       <c r="F4" s="1">
         <v>7</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="12">
         <v>10</v>
       </c>
       <c r="I4" t="s">
@@ -1783,7 +2091,7 @@
       <c r="F5" s="1">
         <v>7</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>15</v>
       </c>
       <c r="I5" t="s">
@@ -2444,15 +2752,15 @@
         <v>2</v>
       </c>
       <c r="I36">
-        <f>FLOOR(I35*$N$34, 1)</f>
+        <f t="shared" ref="I36:I54" si="1">FLOOR(I35*$N$34, 1)</f>
         <v>1100</v>
       </c>
       <c r="J36">
-        <f t="shared" ref="J36:J54" si="1">I36-I35</f>
+        <f t="shared" ref="J36:J54" si="2">I36-I35</f>
         <v>600</v>
       </c>
       <c r="K36">
-        <f t="shared" ref="K36:K54" si="2">I36/J36</f>
+        <f t="shared" ref="K36:K54" si="3">I36/J36</f>
         <v>1.8333333333333333</v>
       </c>
     </row>
@@ -2461,15 +2769,15 @@
         <v>3</v>
       </c>
       <c r="I37">
-        <f>FLOOR(I36*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>2420</v>
       </c>
       <c r="J37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1320</v>
       </c>
       <c r="K37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333333333333</v>
       </c>
     </row>
@@ -2478,15 +2786,15 @@
         <v>4</v>
       </c>
       <c r="I38">
-        <f>FLOOR(I37*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>5324</v>
       </c>
       <c r="J38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2904</v>
       </c>
       <c r="K38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333333333333</v>
       </c>
     </row>
@@ -2495,15 +2803,15 @@
         <v>5</v>
       </c>
       <c r="I39">
-        <f>FLOOR(I38*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>11712</v>
       </c>
       <c r="J39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6388</v>
       </c>
       <c r="K39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.833437695679399</v>
       </c>
     </row>
@@ -2512,15 +2820,15 @@
         <v>6</v>
       </c>
       <c r="I40">
-        <f>FLOOR(I39*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>25766</v>
       </c>
       <c r="J40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14054</v>
       </c>
       <c r="K40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333570513732744</v>
       </c>
     </row>
@@ -2529,15 +2837,15 @@
         <v>7</v>
       </c>
       <c r="I41">
-        <f>FLOOR(I40*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>56685</v>
       </c>
       <c r="J41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30919</v>
       </c>
       <c r="K41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.833338723762088</v>
       </c>
     </row>
@@ -2546,15 +2854,15 @@
         <v>8</v>
       </c>
       <c r="I42">
-        <f>FLOOR(I41*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>124707</v>
       </c>
       <c r="J42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68022</v>
       </c>
       <c r="K42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333333333333</v>
       </c>
     </row>
@@ -2563,15 +2871,15 @@
         <v>9</v>
       </c>
       <c r="I43">
-        <f>FLOOR(I42*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>274355</v>
       </c>
       <c r="J43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>149648</v>
       </c>
       <c r="K43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333355607826365</v>
       </c>
     </row>
@@ -2580,15 +2888,15 @@
         <v>10</v>
       </c>
       <c r="I44">
-        <f>FLOOR(I43*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>603581</v>
       </c>
       <c r="J44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>329226</v>
       </c>
       <c r="K44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333333333333</v>
       </c>
     </row>
@@ -2597,15 +2905,15 @@
         <v>11</v>
       </c>
       <c r="I45">
-        <f>FLOOR(I44*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>1327878</v>
       </c>
       <c r="J45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>724297</v>
       </c>
       <c r="K45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333335634415164</v>
       </c>
     </row>
@@ -2614,15 +2922,15 @@
         <v>12</v>
       </c>
       <c r="I46">
-        <f>FLOOR(I45*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>2921331</v>
       </c>
       <c r="J46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1593453</v>
       </c>
       <c r="K46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333336471172981</v>
       </c>
     </row>
@@ -2631,15 +2939,15 @@
         <v>13</v>
       </c>
       <c r="I47">
-        <f>FLOOR(I46*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>6426928</v>
       </c>
       <c r="J47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3505597</v>
       </c>
       <c r="K47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333808763528</v>
       </c>
     </row>
@@ -2648,15 +2956,15 @@
         <v>14</v>
       </c>
       <c r="I48">
-        <f>FLOOR(I47*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>14139241</v>
       </c>
       <c r="J48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7712313</v>
       </c>
       <c r="K48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333981647271</v>
       </c>
     </row>
@@ -2665,15 +2973,15 @@
         <v>15</v>
       </c>
       <c r="I49">
-        <f>FLOOR(I48*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>31106330</v>
       </c>
       <c r="J49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16967089</v>
       </c>
       <c r="K49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333431562715</v>
       </c>
     </row>
@@ -2682,15 +2990,15 @@
         <v>16</v>
       </c>
       <c r="I50">
-        <f>FLOOR(I49*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>68433926</v>
       </c>
       <c r="J50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37327596</v>
       </c>
       <c r="K50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333333333333</v>
       </c>
     </row>
@@ -2699,15 +3007,15 @@
         <v>17</v>
       </c>
       <c r="I51">
-        <f>FLOOR(I50*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>150554637</v>
       </c>
       <c r="J51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82120711</v>
       </c>
       <c r="K51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.833333335362866</v>
       </c>
     </row>
@@ -2716,15 +3024,15 @@
         <v>18</v>
       </c>
       <c r="I52">
-        <f>FLOOR(I51*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>331220201</v>
       </c>
       <c r="J52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>180665564</v>
       </c>
       <c r="K52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333351783629</v>
       </c>
     </row>
@@ -2733,15 +3041,15 @@
         <v>19</v>
       </c>
       <c r="I53">
-        <f>FLOOR(I52*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>728684442</v>
       </c>
       <c r="J53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>397464241</v>
       </c>
       <c r="K53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333337526583</v>
       </c>
     </row>
@@ -2750,15 +3058,15 @@
         <v>20</v>
       </c>
       <c r="I54">
-        <f>FLOOR(I53*$N$34, 1)</f>
+        <f t="shared" si="1"/>
         <v>1603105772</v>
       </c>
       <c r="J54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>874421330</v>
       </c>
       <c r="K54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8333333337145379</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix plant display levels for level-7 plants
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8E7F2D-454F-4E9E-B588-7920E75355A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEA54D3-1C66-44FE-BABA-E108D257C142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Exp Gain Per Water (Multiple)" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plant Level Tracking'!$A$1:$F$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plant Level Tracking'!$A$1:$F$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Plant Level Tracking Overhaul'!$A$1:$F$21</definedName>
     <definedName name="TotalMultiplier">'Exp Gain Per Water (Multiple)'!$K$2</definedName>
   </definedNames>
@@ -803,7 +803,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:M21"/>
+      <selection activeCell="M14" sqref="M14:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,7 +1842,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F21" xr:uid="{DE796829-81F8-4DDB-A026-28A5EA19C969}">
+  <autoFilter ref="A1:F32" xr:uid="{DE796829-81F8-4DDB-A026-28A5EA19C969}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F32">
       <sortCondition ref="A1:A21"/>
     </sortState>

</xml_diff>

<commit_message>
Add some more flowers uwu
</commit_message>
<xml_diff>
--- a/images/balancing.xlsx
+++ b/images/balancing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\CodeMk2\Python\Discord\Flower\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEA54D3-1C66-44FE-BABA-E108D257C142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA60AC5-66A0-4DD5-B949-577922B9440A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7F91F94-20BF-4783-89AC-9F579D343E4B}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="131">
   <si>
     <t>Plant</t>
   </si>
@@ -405,6 +405,36 @@
   </si>
   <si>
     <t xml:space="preserve">        "18": 7</t>
+  </si>
+  <si>
+    <t>aloe_vera</t>
+  </si>
+  <si>
+    <t>cherry_blossom</t>
+  </si>
+  <si>
+    <t>hyacinth</t>
+  </si>
+  <si>
+    <t>hydrangea</t>
+  </si>
+  <si>
+    <t>lily_of_the_valley</t>
+  </si>
+  <si>
+    <t>moon_flower</t>
+  </si>
+  <si>
+    <t>silent_princess</t>
+  </si>
+  <si>
+    <t>tulip</t>
+  </si>
+  <si>
+    <t>widow_tears</t>
+  </si>
+  <si>
+    <t>Gerti</t>
   </si>
 </sst>
 </file>
@@ -800,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B506C8A2-CFE7-48E4-9F0A-C9D1E39EA76C}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:M19"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,11 +1076,23 @@
       <c r="F6" s="1">
         <v>7</v>
       </c>
+      <c r="H6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6" t="s">
+        <v>122</v>
+      </c>
       <c r="J6" t="s">
         <v>91</v>
       </c>
       <c r="K6" t="s">
         <v>93</v>
+      </c>
+      <c r="L6" t="s">
+        <v>123</v>
+      </c>
+      <c r="M6" t="s">
+        <v>124</v>
       </c>
       <c r="N6" t="s">
         <v>90</v>
@@ -1076,6 +1118,21 @@
       <c r="F7" s="1">
         <v>7</v>
       </c>
+      <c r="I7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7" t="s">
+        <v>127</v>
+      </c>
+      <c r="L7" t="s">
+        <v>128</v>
+      </c>
+      <c r="M7" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1839,6 +1896,105 @@
       </c>
       <c r="F32" s="1">
         <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>129</v>
+      </c>
+      <c r="B41" t="s">
+        <v>130</v>
+      </c>
+      <c r="F41" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>